<commit_message>
update panels datasheet and data entry spreadsheet
</commit_message>
<xml_diff>
--- a/panels/original_datasheets/panels_datasheets.xlsx
+++ b/panels/original_datasheets/panels_datasheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\panels\original_datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015037B-63A8-4393-8A67-CCE6C393113D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EA42AC-5602-4DE3-97BB-A825852BF45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CF3C5995-B323-D84F-AC33-087BF67F67B0}"/>
   </bookViews>
@@ -152,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -210,11 +210,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -263,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,10 +593,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -714,49 +726,76 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,49 +803,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="17"/>
+      <c r="C32" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -815,7 +852,7 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="94" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Bold"&amp;20PANELS Project</oddHeader>
   </headerFooter>
@@ -829,8 +866,8 @@
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>